<commit_message>
12 Jun 2020, push, function call
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/cards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/cards/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{099BF53F-BAAD-2341-BE7F-67453590C817}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCD4A9A-F9DA-7144-AD38-CD19178FCB0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="25220" windowHeight="13140" xr2:uid="{101E426B-AF8F-7E4E-9EB2-B79F93AD1A54}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -408,7 +408,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>43831</v>
+        <v>43936</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -430,7 +430,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>43845</v>
+        <v>43961</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -452,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>43770</v>
+        <v>43910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>